<commit_message>
Utilização de pdf de modo a ser mais fácil de ler
</commit_message>
<xml_diff>
--- a/front-end/front-end-services/Front-end-services.xlsx
+++ b/front-end/front-end-services/Front-end-services.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\front-end\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Ambiente de Trabalho\MESTRADO\2 semestre\Aplicações em Web\aw-project\front-end\front-end-services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E08480-C06D-4C08-96AA-53126A7DA61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763C8C1B-D01F-4E53-BABC-E691AD66CF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF0E2589-CB8B-477F-AEE2-76A16165ADDE}"/>
   </bookViews>
@@ -249,56 +249,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -718,7 +716,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3838574" y="19545299"/>
+          <a:off x="1676399" y="17402174"/>
           <a:ext cx="1457326" cy="2336745"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -838,7 +836,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3476625" y="24669750"/>
+          <a:off x="1314450" y="27298650"/>
           <a:ext cx="2126552" cy="1743076"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1301,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832E6391-5178-4AA5-93E0-67A87F0C74F9}">
   <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,303 +1325,302 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="14" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="15"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="14" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="15"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="14" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="15"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8" ht="189.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="15"/>
+      <c r="F6" s="12"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="14" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="15"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="2:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="14" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="15"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="14" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="15"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="2:8" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="14" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="15"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="14" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="14" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="14" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="14" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="14" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="14" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="14" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="189.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="14" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="14" t="s">
+      <c r="B21" s="15"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="14" t="s">
+      <c r="B22" s="15"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="14" t="s">
+      <c r="B23" s="15"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="14" t="s">
+      <c r="B24" s="15"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="14" t="s">
+    <row r="25" spans="2:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14" t="s">
+      <c r="B26" s="15"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="14" t="s">
+      <c r="B27" s="15"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="14" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="14" t="s">
+      <c r="B29" s="11"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="14" t="s">
+      <c r="C30" s="8"/>
+      <c r="D30" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="14" t="s">
+      <c r="B31" s="11"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="14" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="14" t="s">
+      <c r="B33" s="15"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="14" t="s">
+      <c r="B34" s="15"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="14" t="s">
+      <c r="B35" s="15"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="14" t="s">
+      <c r="B36" s="11"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="5" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="C32:C36"/>
     <mergeCell ref="F3:F10"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B14:B29"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C3:C5"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B3:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>